<commit_message>
Regression API Suite for PO
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A28DD4B-FFE8-4BC3-BF81-E97C4900E444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5A28DD4B-FFE8-4BC3-BF81-E97C4900E444}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2D3706E6-F74E-412D-B856-F4DCD436F230}"/>
+    <workbookView activeTab="2" windowHeight="11040" windowWidth="20730" xWindow="-120" xr2:uid="{2D3706E6-F74E-412D-B856-F4DCD436F230}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="POHeader" sheetId="4" r:id="rId1"/>
-    <sheet name="Multiple PO Line" sheetId="5" r:id="rId2"/>
-    <sheet name="POReceipt" sheetId="1" r:id="rId3"/>
-    <sheet name="POAuthorization" sheetId="2" r:id="rId4"/>
-    <sheet name="POAPMatch" sheetId="3" r:id="rId5"/>
-    <sheet name="CloseAPBatch" sheetId="7" r:id="rId6"/>
-    <sheet name="SYDATAD" sheetId="6" r:id="rId7"/>
+    <sheet name="POHeader" r:id="rId1" sheetId="4"/>
+    <sheet name="Multiple PO Line" r:id="rId2" sheetId="5"/>
+    <sheet name="POReceipt" r:id="rId3" sheetId="1"/>
+    <sheet name="POAuthorization" r:id="rId4" sheetId="2"/>
+    <sheet name="POAPMatch" r:id="rId5" sheetId="3"/>
+    <sheet name="CloseAPBatch" r:id="rId6" sheetId="7"/>
+    <sheet name="SYDATAD" r:id="rId7" sheetId="6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -208,7 +208,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +230,150 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,7 +390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -251,21 +398,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="28">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="10" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="12" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="14" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="20" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="22" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="24" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -282,10 +489,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -320,7 +527,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -372,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -483,21 +690,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -514,7 +721,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -566,14 +773,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0343F24-40D4-4440-9D54-55228C8E570C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0343F24-40D4-4440-9D54-55228C8E570C}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -582,12 +789,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -651,13 +858,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FBD9E7-0F05-4B09-A258-92FDFEAF64E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FBD9E7-0F05-4B09-A258-92FDFEAF64E9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -666,10 +873,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,13 +1018,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C65B3F5-9AF7-4EF8-99A3-B6CFE9D357A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C65B3F5-9AF7-4EF8-99A3-B6CFE9D357A8}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -826,16 +1033,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.8046875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.84375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.15234375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.1953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.3828125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.3828125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.92578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.83984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -979,13 +1187,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3140E94-A77F-4ADA-B38D-721536A01E45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3140E94-A77F-4ADA-B38D-721536A01E45}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -994,9 +1202,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1063,12 +1271,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07130A80-619A-4C08-AB25-C355965EA3FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07130A80-619A-4C08-AB25-C355965EA3FB}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1112,13 +1320,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ED1D65-0BA8-453D-8E93-E71AD9B6AEB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ED1D65-0BA8-453D-8E93-E71AD9B6AEB2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1127,11 +1335,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,13 +1377,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA944A1-FC72-490D-881A-48958A944509}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA944A1-FC72-490D-881A-48958A944509}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1184,8 +1392,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,6 +1413,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated SYDATA Regression TC
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
@@ -211,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="75" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +230,294 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -390,7 +678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -434,11 +722,83 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -465,8 +825,56 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="22" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="24" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="25" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="26" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="28" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="29" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="30" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="31" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="32" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="34" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="35" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="36" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="37" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="38" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="40" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="42" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="43" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="44" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="46" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="48" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="50" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="51" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="52" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="53" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="54" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="55" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="56" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="57" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="58" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="59" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="29" fillId="0" fontId="60" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="61" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="62" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="63" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="64" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="65" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="66" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="67" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="68" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="69" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="70" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="71" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="72" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="74" fillId="0" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>

</xml_diff>

<commit_message>
Fixed data issue related to unique ID generation
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/SYDATA-POtoPOAP Match_AutomationOrg.xlsx
@@ -211,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="285" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +230,1554 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -390,7 +1938,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="142">
     <border>
       <left/>
       <right/>
@@ -434,11 +1982,398 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="286">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -465,8 +2400,266 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="22" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="24" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="25" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="26" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="28" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="29" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="30" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="31" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="32" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="34" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="35" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="36" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="37" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="38" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="40" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="42" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="43" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="44" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="46" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="48" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="50" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="51" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="52" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="53" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="54" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="55" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="56" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="57" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="58" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="59" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="29" fillId="0" fontId="60" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="61" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="62" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="63" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="64" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="65" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="66" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="67" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="68" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="69" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="70" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="71" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="72" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="73" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="74" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="75" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="76" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="77" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="78" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="79" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="80" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="81" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="82" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="83" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="84" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="85" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="86" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="87" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="88" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="89" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="90" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="91" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="92" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="93" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="94" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="95" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="96" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="97" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="98" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="99" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="100" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="101" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="102" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="103" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="104" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="105" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="106" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="107" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="108" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="109" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="110" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="111" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="112" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="113" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="114" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="115" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="116" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="117" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="118" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="119" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="120" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="121" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="122" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="123" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="124" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="125" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="126" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="127" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="128" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="129" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="130" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="131" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="132" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="133" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="134" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="135" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="136" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="137" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="68" fillId="0" fontId="138" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="139" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="69" fillId="0" fontId="140" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="141" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="142" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="143" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="144" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="145" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="72" fillId="0" fontId="146" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="147" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="73" fillId="0" fontId="148" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="149" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="74" fillId="0" fontId="150" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="151" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="75" fillId="0" fontId="152" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="153" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="154" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="155" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="156" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="157" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="78" fillId="0" fontId="158" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="159" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="79" fillId="0" fontId="160" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="161" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="80" fillId="0" fontId="162" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="163" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="81" fillId="0" fontId="164" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="165" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="82" fillId="0" fontId="166" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="167" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="83" fillId="0" fontId="168" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="169" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="84" fillId="0" fontId="170" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="171" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="85" fillId="0" fontId="172" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="173" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="86" fillId="0" fontId="174" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="175" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="87" fillId="0" fontId="176" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="177" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="88" fillId="0" fontId="178" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="179" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="89" fillId="0" fontId="180" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="181" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="90" fillId="0" fontId="182" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="183" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="91" fillId="0" fontId="184" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="185" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="92" fillId="0" fontId="186" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="187" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="93" fillId="0" fontId="188" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="189" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="94" fillId="0" fontId="190" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="191" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="95" fillId="0" fontId="192" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="193" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="96" fillId="0" fontId="194" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="195" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="97" fillId="0" fontId="196" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="197" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="98" fillId="0" fontId="198" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="199" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="99" fillId="0" fontId="200" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="201" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="100" fillId="0" fontId="202" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="203" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="101" fillId="0" fontId="204" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="205" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="102" fillId="0" fontId="206" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="207" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="103" fillId="0" fontId="208" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="209" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="104" fillId="0" fontId="210" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="211" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="105" fillId="0" fontId="212" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="213" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="106" fillId="0" fontId="214" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="215" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="107" fillId="0" fontId="216" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="217" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="108" fillId="0" fontId="218" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="219" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="109" fillId="0" fontId="220" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="221" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="110" fillId="0" fontId="222" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="223" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="111" fillId="0" fontId="224" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="225" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="112" fillId="0" fontId="226" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="227" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="113" fillId="0" fontId="228" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="229" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="114" fillId="0" fontId="230" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="231" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="115" fillId="0" fontId="232" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="233" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="116" fillId="0" fontId="234" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="235" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="117" fillId="0" fontId="236" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="237" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="118" fillId="0" fontId="238" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="239" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="119" fillId="0" fontId="240" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="241" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="120" fillId="0" fontId="242" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="243" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="121" fillId="0" fontId="244" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="245" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="122" fillId="0" fontId="246" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="247" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="123" fillId="0" fontId="248" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="249" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="124" fillId="0" fontId="250" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="251" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="125" fillId="0" fontId="252" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="253" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="126" fillId="0" fontId="254" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="255" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="127" fillId="0" fontId="256" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="257" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="128" fillId="0" fontId="258" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="259" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="129" fillId="0" fontId="260" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="261" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="130" fillId="0" fontId="262" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="263" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="131" fillId="0" fontId="264" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="265" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="132" fillId="0" fontId="266" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="267" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="133" fillId="0" fontId="268" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="269" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="134" fillId="0" fontId="270" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="271" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="135" fillId="0" fontId="272" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="273" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="136" fillId="0" fontId="274" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="275" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="137" fillId="0" fontId="276" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="277" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="138" fillId="0" fontId="278" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="279" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="139" fillId="0" fontId="280" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="281" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="140" fillId="0" fontId="282" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="283" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="284" fillId="0" borderId="141" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>

</xml_diff>